<commit_message>
update header and note
</commit_message>
<xml_diff>
--- a/pjets/expdata/20001.xlsx
+++ b/pjets/expdata/20001.xlsx
@@ -1,56 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yiyu/Google Drive/ing/jefferson lab/scholarship/monte carlo/fitpack2/database/pjet/expdata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32AACCB-DC4F-A44C-B04D-517D1A9AEEED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="25600" windowHeight="14900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="17020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
+  <si>
+    <t>idx</t>
+  </si>
   <si>
     <t>col</t>
   </si>
   <si>
+    <t>particles-in</t>
+  </si>
+  <si>
     <t>RS</t>
   </si>
   <si>
+    <t>pt-min</t>
+  </si>
+  <si>
+    <t>pt-max</t>
+  </si>
+  <si>
     <t>pT</t>
   </si>
   <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>eta-min</t>
+  </si>
+  <si>
+    <t>eta-max</t>
+  </si>
+  <si>
+    <t>cone-radius</t>
+  </si>
+  <si>
     <t>obs</t>
   </si>
   <si>
     <t>value</t>
   </si>
   <si>
-    <t>tau</t>
-  </si>
-  <si>
-    <t>idx</t>
-  </si>
-  <si>
     <t>stat_u</t>
   </si>
   <si>
+    <t>sys_c</t>
+  </si>
+  <si>
     <t>star</t>
   </si>
   <si>
@@ -58,58 +68,378 @@
   </si>
   <si>
     <t>&lt;a_ll&gt;</t>
-  </si>
-  <si>
-    <t>eta_min</t>
-  </si>
-  <si>
-    <t>eta_max</t>
-  </si>
-  <si>
-    <t>sys_c</t>
-  </si>
-  <si>
-    <t>cone_radius</t>
-  </si>
-  <si>
-    <t>pt_max</t>
-  </si>
-  <si>
-    <t>pt_min</t>
-  </si>
-  <si>
-    <t>particles_in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="17"/>
       <color rgb="FF000000"/>
       <name val="Gabriola"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="26"/>
       <color rgb="FF000000"/>
       <name val="Gabriola"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -117,9 +447,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -127,17 +699,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -186,7 +802,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -219,26 +835,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -271,23 +870,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -429,87 +1011,81 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.71120689655172" defaultRowHeight="24.4"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="2" max="2" width="10.2844827586207" customWidth="1"/>
+    <col min="3" max="3" width="13.8534482758621" customWidth="1"/>
+    <col min="4" max="8" width="10.2844827586207" customWidth="1"/>
+    <col min="9" max="9" width="14.8534482758621" customWidth="1"/>
+    <col min="10" max="11" width="15.5689655172414" customWidth="1"/>
+    <col min="12" max="12" width="7.85344827586207" customWidth="1"/>
+    <col min="13" max="14" width="17" customWidth="1"/>
     <col min="15" max="16" width="16" customWidth="1"/>
-    <col min="17" max="20" width="10.28515625" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="1027" width="10.28515625" customWidth="1"/>
+    <col min="17" max="20" width="10.2844827586207" customWidth="1"/>
+    <col min="21" max="21" width="11.8534482758621" customWidth="1"/>
+    <col min="22" max="22" width="14.1422413793103" customWidth="1"/>
+    <col min="23" max="1027" width="10.2844827586207" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" ht="35.6" spans="1:22">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -519,15 +1095,15 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" ht="35.6" spans="1:22">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>200</v>
@@ -543,7 +1119,7 @@
       </c>
       <c r="H2" s="1">
         <f t="shared" ref="H2:H7" si="0">2*G2/D2</f>
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="I2" s="1">
         <v>0.2</v>
@@ -555,16 +1131,16 @@
         <v>0.4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M2" s="1">
-        <v>1.4E-2</v>
+        <v>0.014</v>
       </c>
       <c r="N2" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0.022</v>
       </c>
       <c r="O2" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -574,15 +1150,15 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" ht="35.6" spans="1:22">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
         <v>200</v>
@@ -598,7 +1174,7 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" si="0"/>
-        <v>6.8000000000000005E-2</v>
+        <v>0.068</v>
       </c>
       <c r="I3" s="1">
         <v>0.2</v>
@@ -610,16 +1186,16 @@
         <v>0.4</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M3" s="1">
-        <v>-6.6000000000000003E-2</v>
+        <v>-0.066</v>
       </c>
       <c r="N3" s="1">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="O3" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0.022</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -629,15 +1205,15 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" ht="35.6" spans="1:22">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
         <v>200</v>
@@ -646,14 +1222,14 @@
         <v>7.6</v>
       </c>
       <c r="F4" s="1">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="G4" s="1">
-        <v>8.3000000000000007</v>
+        <v>8.3</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
+        <v>0.083</v>
       </c>
       <c r="I4" s="1">
         <v>0.2</v>
@@ -665,16 +1241,16 @@
         <v>0.4</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M4" s="1">
-        <v>-1.9E-2</v>
+        <v>-0.019</v>
       </c>
       <c r="N4" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>0.029</v>
       </c>
       <c r="O4" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -684,31 +1260,31 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" ht="35.6" spans="1:22">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1">
         <v>200</v>
       </c>
       <c r="E5" s="1">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="F5" s="1">
         <v>11.4</v>
       </c>
       <c r="G5" s="1">
-        <v>10.199999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>0.10199999999999999</v>
+        <v>0.102</v>
       </c>
       <c r="I5" s="1">
         <v>0.2</v>
@@ -720,16 +1296,16 @@
         <v>0.4</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M5" s="1">
-        <v>-1.4999999999999999E-2</v>
+        <v>-0.015</v>
       </c>
       <c r="N5" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>0.038</v>
       </c>
       <c r="O5" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -739,15 +1315,15 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" ht="35.6" spans="1:22">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1">
         <v>200</v>
@@ -775,16 +1351,16 @@
         <v>0.4</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M6" s="1">
-        <v>-8.9999999999999993E-3</v>
+        <v>-0.009</v>
       </c>
       <c r="N6" s="1">
-        <v>5.1999999999999998E-2</v>
+        <v>0.052</v>
       </c>
       <c r="O6" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -794,15 +1370,15 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" ht="35.6" spans="1:22">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1">
         <v>200</v>
@@ -830,16 +1406,16 @@
         <v>0.4</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M7" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
       <c r="N7" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="O7" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -849,7 +1425,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" ht="35.6" spans="2:16">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -863,7 +1439,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" ht="35.6" spans="2:16">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -877,7 +1453,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" ht="35.6" spans="2:16">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -891,7 +1467,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" ht="35.6" spans="2:16">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -905,7 +1481,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" ht="35.6" spans="2:16">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -919,7 +1495,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" ht="35.6" spans="2:16">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -933,7 +1509,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" ht="35.6" spans="2:16">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -947,7 +1523,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" ht="35.6" spans="2:16">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -961,7 +1537,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:22" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" ht="35.6" spans="2:16">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -975,7 +1551,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="2:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" ht="35.6" spans="2:16">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -989,7 +1565,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="2:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" ht="35.6" spans="2:16">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1003,7 +1579,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" ht="35.6" spans="2:16">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1018,7 +1594,8 @@
       <c r="P19" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>